<commit_message>
[update] ExcelData of weapon
</commit_message>
<xml_diff>
--- a/NoAlly/Assets/Excel/Weapon/WeaponTable.xlsx
+++ b/NoAlly/Assets/Excel/Weapon/WeaponTable.xlsx
@@ -1,39 +1,32 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25629"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25726"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\vantan\2DActionGameA\NoAlly\Assets\Excel\Weapon\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2D68A469-9EFB-4368-9510-9F127911D6DA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A771A1CF-9473-403C-8A6D-224726931996}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="7164" yWindow="2040" windowWidth="17280" windowHeight="8964" xr2:uid="{945BC0FA-4342-4D63-B007-195514FBD902}"/>
+    <workbookView xWindow="5556" yWindow="2124" windowWidth="17280" windowHeight="8844" activeTab="1" xr2:uid="{945BC0FA-4342-4D63-B007-195514FBD902}"/>
   </bookViews>
   <sheets>
     <sheet name="WeaponData" sheetId="1" r:id="rId1"/>
+    <sheet name="ElementWeaponData" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
-      </xcalcf:calcFeatures>
-    </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="9">
   <si>
     <t>Name</t>
     <phoneticPr fontId="1"/>
@@ -434,8 +427,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{99084F10-4981-48C2-A3A0-3FB9037EE30F}">
   <dimension ref="A1:E5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:E1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18" x14ac:dyDescent="0.45"/>
@@ -536,4 +529,111 @@
   <phoneticPr fontId="1"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{75E8A9F5-7443-40B4-93D6-047D73F452E3}">
+  <dimension ref="A1:E5"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B5" sqref="B5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="18" x14ac:dyDescent="0.45"/>
+  <cols>
+    <col min="2" max="2" width="10.3984375" customWidth="1"/>
+    <col min="3" max="3" width="10.8984375" customWidth="1"/>
+    <col min="4" max="4" width="9.5" customWidth="1"/>
+    <col min="5" max="5" width="11.69921875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A2" t="s">
+        <v>5</v>
+      </c>
+      <c r="B2">
+        <v>3</v>
+      </c>
+      <c r="C2">
+        <v>0</v>
+      </c>
+      <c r="D2">
+        <v>5</v>
+      </c>
+      <c r="E2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A3" t="s">
+        <v>6</v>
+      </c>
+      <c r="B3">
+        <v>2</v>
+      </c>
+      <c r="C3">
+        <v>0</v>
+      </c>
+      <c r="D3">
+        <v>0</v>
+      </c>
+      <c r="E3">
+        <v>5.5</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A4" t="s">
+        <v>7</v>
+      </c>
+      <c r="B4">
+        <v>3</v>
+      </c>
+      <c r="C4">
+        <v>0</v>
+      </c>
+      <c r="D4">
+        <v>0</v>
+      </c>
+      <c r="E4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A5" t="s">
+        <v>8</v>
+      </c>
+      <c r="B5">
+        <v>3.5</v>
+      </c>
+      <c r="C5">
+        <v>6</v>
+      </c>
+      <c r="D5">
+        <v>0</v>
+      </c>
+      <c r="E5">
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="1"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>